<commit_message>
working connector w/ data
</commit_message>
<xml_diff>
--- a/bosch wrangled.xlsx
+++ b/bosch wrangled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cerda\Documents\WrWx\Python Files\WranglesPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE92524-B70C-4106-BABC-83E59C56B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175ACB4-1193-4D52-A2FC-F1B53FCFDD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28410" yWindow="495" windowWidth="26070" windowHeight="12405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>15.74 USD</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>758.53 USD</t>
   </si>
   <si>
@@ -355,9 +352,6 @@
     <t>92.24 USD</t>
   </si>
   <si>
-    <t>5lb</t>
-  </si>
-  <si>
     <t>5 lb</t>
   </si>
   <si>
@@ -404,6 +398,12 @@
   </si>
   <si>
     <t>Family2</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>VOLT</t>
   </si>
 </sst>
 </file>
@@ -531,6 +531,8 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -582,8 +584,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -649,9 +649,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:R11">
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SKU"/>
-    <tableColumn id="19" xr3:uid="{3AEF2B56-AF63-4F9E-97F3-06959DEEDAD0}" name="family" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{296431EE-1B5E-4419-91E7-C693FC8FD5E5}" name="categories" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{E911FBD2-5E9E-41BE-918F-574A5E6949CE}" name="groups" dataDxfId="0"/>
+    <tableColumn id="19" xr3:uid="{3AEF2B56-AF63-4F9E-97F3-06959DEEDAD0}" name="family" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{296431EE-1B5E-4419-91E7-C693FC8FD5E5}" name="categories" dataDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{E911FBD2-5E9E-41BE-918F-574A5E6949CE}" name="groups" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="BOSCH DESCRIPTION"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Attributes"/>
@@ -660,12 +660,12 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tool Weight"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Tool Length"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Voltage"/>
-    <tableColumn id="16" xr3:uid="{9F0F916A-25B4-4489-9343-C14910BDEFB9}" name="Current Type" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{9F0F916A-25B4-4489-9343-C14910BDEFB9}" name="Current Type" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="BOSCH CATEGORY"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Item"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Family2"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Category"/>
-    <tableColumn id="18" xr3:uid="{0581FE27-2280-4A5C-95DF-B07FF7858EBF}" name="USD" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{0581FE27-2280-4A5C-95DF-B07FF7858EBF}" name="Price" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -869,7 +869,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="536" row="5">
+  <wetp:taskpane dockstate="right" visibility="0" width="457" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -920,13 +920,13 @@
         <v>82</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -962,13 +962,13 @@
         <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
@@ -1000,13 +1000,13 @@
         <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>94</v>
@@ -1038,7 +1038,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -1059,7 +1059,7 @@
         <v>24</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>97</v>
@@ -1080,7 +1080,7 @@
         <v>27</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>12</v>
@@ -1115,10 +1115,10 @@
         <v>32</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>94</v>
@@ -1136,7 +1136,7 @@
         <v>27</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>12</v>
@@ -1168,13 +1168,13 @@
         <v>37</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>94</v>
@@ -1192,7 +1192,7 @@
         <v>40</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>12</v>
@@ -1224,13 +1224,13 @@
         <v>45</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>94</v>
@@ -1248,7 +1248,7 @@
         <v>40</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>12</v>
@@ -1302,7 +1302,7 @@
         <v>27</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>12</v>
@@ -1358,7 +1358,7 @@
         <v>59</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -1414,7 +1414,7 @@
         <v>59</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1428,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>12</v>
@@ -1446,13 +1446,13 @@
         <v>68</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>95</v>
@@ -1470,7 +1470,7 @@
         <v>40</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1484,7 +1484,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
@@ -1498,13 +1498,13 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="L11" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>95</v>
@@ -1522,7 +1522,7 @@
         <v>40</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2521,7 +2521,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2569,7 +2569,7 @@
         <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>